<commit_message>
added the GUI component
</commit_message>
<xml_diff>
--- a/trading_synthesis.xlsx
+++ b/trading_synthesis.xlsx
@@ -510,10 +510,10 @@
         <v>0.64</v>
       </c>
       <c r="E2" t="n">
-        <v>125.82</v>
+        <v>123.64</v>
       </c>
       <c r="F2" t="n">
-        <v>36.51</v>
+        <v>36.52</v>
       </c>
       <c r="G2" t="n">
         <v>38.13</v>
@@ -522,7 +522,7 @@
         <v>0.21</v>
       </c>
       <c r="I2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr"/>
     </row>
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>194.62</v>
+        <v>193.5</v>
       </c>
       <c r="E3" t="n">
-        <v>114.3</v>
+        <v>101.94</v>
       </c>
       <c r="F3" t="n">
-        <v>63.32</v>
+        <v>63.25</v>
       </c>
       <c r="G3" t="n">
         <v>78.33</v>
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1373.21</v>
+        <v>1372.45</v>
       </c>
       <c r="E4" t="n">
-        <v>-172.97</v>
+        <v>-173.54</v>
       </c>
       <c r="F4" t="n">
-        <v>79.42</v>
+        <v>79.41</v>
       </c>
       <c r="G4" t="n">
         <v>79.14</v>
@@ -592,7 +592,11 @@
       <c r="I4" t="n">
         <v>0.37</v>
       </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -711,13 +715,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>108840.01</v>
+        <v>107702.3</v>
       </c>
       <c r="E8" t="n">
-        <v>129.95</v>
+        <v>127.18</v>
       </c>
       <c r="F8" t="n">
-        <v>79.75</v>
+        <v>79.72</v>
       </c>
       <c r="G8" t="n">
         <v>82.95999999999999</v>
@@ -745,13 +749,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>76.81</v>
+        <v>76.76000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>140.52</v>
+        <v>139.9</v>
       </c>
       <c r="F9" t="n">
-        <v>69.95999999999999</v>
+        <v>69.95</v>
       </c>
       <c r="G9" t="n">
         <v>72.12</v>
@@ -779,13 +783,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>241.78</v>
+        <v>244.23</v>
       </c>
       <c r="E10" t="n">
-        <v>211.72</v>
+        <v>219.96</v>
       </c>
       <c r="F10" t="n">
-        <v>87.09999999999999</v>
+        <v>87.09</v>
       </c>
       <c r="G10" t="n">
         <v>90.81</v>
@@ -813,10 +817,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23.3</v>
+        <v>23.27</v>
       </c>
       <c r="E11" t="n">
-        <v>-117.29</v>
+        <v>-117.47</v>
       </c>
       <c r="F11" t="n">
         <v>43.12</v>
@@ -847,13 +851,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1211.57</v>
+        <v>1208.15</v>
       </c>
       <c r="E12" t="n">
-        <v>148.7</v>
+        <v>148.84</v>
       </c>
       <c r="F12" t="n">
-        <v>90.89</v>
+        <v>90.87</v>
       </c>
       <c r="G12" t="n">
         <v>91.37</v>
@@ -881,13 +885,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>460.69</v>
+        <v>459.83</v>
       </c>
       <c r="E13" t="n">
-        <v>142.79</v>
+        <v>143.35</v>
       </c>
       <c r="F13" t="n">
-        <v>63.18</v>
+        <v>63.16</v>
       </c>
       <c r="G13" t="n">
         <v>76.86</v>
@@ -915,16 +919,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>257.3</v>
+        <v>253.36</v>
       </c>
       <c r="E14" t="n">
-        <v>191.22</v>
+        <v>184.03</v>
       </c>
       <c r="F14" t="n">
-        <v>49.23</v>
+        <v>49.16</v>
       </c>
       <c r="G14" t="n">
-        <v>52.3</v>
+        <v>52.29</v>
       </c>
       <c r="H14" t="n">
         <v>0.59</v>
@@ -949,13 +953,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>279.23</v>
+        <v>277.42</v>
       </c>
       <c r="E15" t="n">
-        <v>118.65</v>
+        <v>114.83</v>
       </c>
       <c r="F15" t="n">
-        <v>62.26</v>
+        <v>62.22</v>
       </c>
       <c r="G15" t="n">
         <v>79.55</v>
@@ -983,19 +987,19 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1.66</v>
+        <v>1.53</v>
       </c>
       <c r="E16" t="n">
-        <v>128.41</v>
+        <v>112.28</v>
       </c>
       <c r="F16" t="n">
-        <v>8.32</v>
+        <v>8.25</v>
       </c>
       <c r="G16" t="n">
         <v>12.81</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="I16" t="n">
         <v>-0.3</v>
@@ -1088,16 +1092,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>8770.450000000001</v>
+        <v>8744.559999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>115.95</v>
+        <v>107.32</v>
       </c>
       <c r="F2" t="n">
-        <v>63.24</v>
+        <v>63.21</v>
       </c>
       <c r="G2" t="n">
-        <v>67.06999999999999</v>
+        <v>67.06</v>
       </c>
       <c r="H2" t="n">
         <v>0.01</v>
@@ -1143,7 +1147,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45804</v>
+        <v>45805</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1156,28 +1160,28 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>109.09</v>
+        <v>108.57</v>
       </c>
       <c r="E4" t="n">
-        <v>122.35</v>
+        <v>110.81</v>
       </c>
       <c r="F4" t="n">
-        <v>52.72</v>
+        <v>52.27</v>
       </c>
       <c r="G4" t="n">
-        <v>68.45</v>
+        <v>67.69</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.86</v>
+        <v>-0.77</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.59</v>
+        <v>-0.63</v>
       </c>
       <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45804</v>
+        <v>45805</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1190,28 +1194,28 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4.49</v>
+        <v>4.09</v>
       </c>
       <c r="E5" t="n">
-        <v>192.43</v>
+        <v>160.79</v>
       </c>
       <c r="F5" t="n">
-        <v>14.91</v>
+        <v>16.2</v>
       </c>
       <c r="G5" t="n">
-        <v>22.4</v>
+        <v>21.68</v>
       </c>
       <c r="H5" t="n">
-        <v>0.38</v>
+        <v>0.55</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.96</v>
+        <v>-0.92</v>
       </c>
       <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45804</v>
+        <v>45805</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1224,19 +1228,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9.550000000000001</v>
+        <v>9.83</v>
       </c>
       <c r="E6" t="n">
-        <v>128.11</v>
+        <v>168.8</v>
       </c>
       <c r="F6" t="n">
-        <v>31.76</v>
+        <v>32.06</v>
       </c>
       <c r="G6" t="n">
-        <v>34.84</v>
+        <v>34.6</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
       <c r="I6" t="n">
         <v>-0.28</v>
@@ -1254,7 +1258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1332,10 +1336,10 @@
         <v>0.64</v>
       </c>
       <c r="E2" t="n">
-        <v>-104.76</v>
+        <v>-111.13</v>
       </c>
       <c r="F2" t="n">
-        <v>51.28</v>
+        <v>51.31</v>
       </c>
       <c r="G2" t="n">
         <v>48.75</v>
@@ -1366,10 +1370,10 @@
         <v>1.13</v>
       </c>
       <c r="E3" t="n">
-        <v>-101.63</v>
+        <v>-104.44</v>
       </c>
       <c r="F3" t="n">
-        <v>70.45</v>
+        <v>70.48</v>
       </c>
       <c r="G3" t="n">
         <v>54.19</v>
@@ -1388,37 +1392,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GBPUSD=X</t>
+          <t>EURJPY=X</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.35</v>
+        <v>163.67</v>
       </c>
       <c r="E4" t="n">
-        <v>-117.79</v>
+        <v>101.23</v>
       </c>
       <c r="F4" t="n">
-        <v>81.42</v>
+        <v>34.74</v>
       </c>
       <c r="G4" t="n">
-        <v>67.97</v>
+        <v>42.61</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3</v>
+        <v>0.21</v>
       </c>
       <c r="I4" t="n">
-        <v>0.99</v>
+        <v>-0.63</v>
       </c>
       <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45805.54166666666</v>
+        <v>45805.5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1427,66 +1431,66 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>^SSMI</t>
+          <t>GBPUSD=X</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>12206.74</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
-        <v>-100.97</v>
+        <v>-115.83</v>
       </c>
       <c r="F5" t="n">
-        <v>81.59</v>
+        <v>81.53</v>
       </c>
       <c r="G5" t="n">
-        <v>77.36</v>
+        <v>67.97</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.06</v>
+        <v>0.3</v>
       </c>
       <c r="I5" t="n">
-        <v>0.67</v>
+        <v>0.99</v>
       </c>
       <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45804.5625</v>
+        <v>45805.5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LIT</t>
+          <t>USDJPY=X</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>37.31</v>
+        <v>144.57</v>
       </c>
       <c r="E6" t="n">
-        <v>-116.74</v>
+        <v>107.88</v>
       </c>
       <c r="F6" t="n">
-        <v>64.64</v>
+        <v>27.72</v>
       </c>
       <c r="G6" t="n">
-        <v>48.12</v>
+        <v>43.81</v>
       </c>
       <c r="H6" t="n">
-        <v>0.42</v>
+        <v>-0.31</v>
       </c>
       <c r="I6" t="n">
-        <v>0.97</v>
+        <v>-1</v>
       </c>
       <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45804.5625</v>
+        <v>45805.5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1495,66 +1499,66 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USO</t>
+          <t>USDILS=X</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>67.29000000000001</v>
+        <v>3.51</v>
       </c>
       <c r="E7" t="n">
-        <v>-105.45</v>
+        <v>-108.46</v>
       </c>
       <c r="F7" t="n">
-        <v>48.19</v>
+        <v>36.85</v>
       </c>
       <c r="G7" t="n">
-        <v>39.4</v>
+        <v>28.97</v>
       </c>
       <c r="H7" t="n">
-        <v>0.66</v>
+        <v>-0.05</v>
       </c>
       <c r="I7" t="n">
-        <v>0.03</v>
+        <v>0.51</v>
       </c>
       <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45805.5</v>
+        <v>45805.54166666666</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>DOT-USD</t>
+          <t>^SSMI</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4.64</v>
+        <v>12199.01</v>
       </c>
       <c r="E8" t="n">
-        <v>155.92</v>
+        <v>-108.22</v>
       </c>
       <c r="F8" t="n">
-        <v>29.16</v>
+        <v>81.56</v>
       </c>
       <c r="G8" t="n">
-        <v>34.45</v>
+        <v>77.36</v>
       </c>
       <c r="H8" t="n">
-        <v>0.11</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.55</v>
+        <v>0.67</v>
       </c>
       <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45804.5625</v>
+        <v>45805.39583333334</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1563,28 +1567,198 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>LIT</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>37.08</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-132.36</v>
+      </c>
+      <c r="F9" t="n">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>GM</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>49.09</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-108.24</v>
-      </c>
-      <c r="F9" t="n">
-        <v>61.77</v>
-      </c>
-      <c r="G9" t="n">
-        <v>42.94</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>48.47</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-149.89</v>
+      </c>
+      <c r="F10" t="n">
+        <v>62.58</v>
+      </c>
+      <c r="G10" t="n">
+        <v>43.7</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>LYV</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>141.87</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-119.52</v>
+      </c>
+      <c r="F11" t="n">
+        <v>87.22</v>
+      </c>
+      <c r="G11" t="n">
+        <v>73.89</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-107.21</v>
+      </c>
+      <c r="F12" t="n">
+        <v>67.13</v>
+      </c>
+      <c r="G12" t="n">
+        <v>46.36</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BITF</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-172.7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>75.61</v>
+      </c>
+      <c r="G13" t="n">
+        <v>55.51</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ARBK</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-104.58</v>
+      </c>
+      <c r="F14" t="n">
+        <v>66.52</v>
+      </c>
+      <c r="G14" t="n">
+        <v>51.41</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
addition of the bat launching script
</commit_message>
<xml_diff>
--- a/trading_synthesis.xlsx
+++ b/trading_synthesis.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,10 +510,10 @@
         <v>0.64</v>
       </c>
       <c r="E2" t="n">
-        <v>123.64</v>
+        <v>127.25</v>
       </c>
       <c r="F2" t="n">
-        <v>36.52</v>
+        <v>36.55</v>
       </c>
       <c r="G2" t="n">
         <v>38.13</v>
@@ -541,19 +541,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>193.5</v>
+        <v>195.73</v>
       </c>
       <c r="E3" t="n">
-        <v>101.94</v>
+        <v>133.17</v>
       </c>
       <c r="F3" t="n">
-        <v>63.25</v>
+        <v>63.39</v>
       </c>
       <c r="G3" t="n">
         <v>78.33</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.98</v>
+        <v>-0.97</v>
       </c>
       <c r="I3" t="n">
         <v>-0.68</v>
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1372.45</v>
+        <v>1373.28</v>
       </c>
       <c r="E4" t="n">
-        <v>-173.54</v>
+        <v>-167.35</v>
       </c>
       <c r="F4" t="n">
-        <v>79.41</v>
+        <v>79.42</v>
       </c>
       <c r="G4" t="n">
         <v>79.14</v>
@@ -616,10 +616,10 @@
         <v>7.19</v>
       </c>
       <c r="E5" t="n">
-        <v>-124.85</v>
+        <v>-122.12</v>
       </c>
       <c r="F5" t="n">
-        <v>63.93</v>
+        <v>63.91</v>
       </c>
       <c r="G5" t="n">
         <v>63.03</v>
@@ -647,13 +647,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>24752.45</v>
+        <v>24699.5</v>
       </c>
       <c r="E6" t="n">
-        <v>138.3</v>
+        <v>136.07</v>
       </c>
       <c r="F6" t="n">
-        <v>69.7</v>
+        <v>69.68000000000001</v>
       </c>
       <c r="G6" t="n">
         <v>83.43000000000001</v>
@@ -681,19 +681,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2670.15</v>
+        <v>2720.64</v>
       </c>
       <c r="E7" t="n">
-        <v>137.38</v>
+        <v>167.67</v>
       </c>
       <c r="F7" t="n">
-        <v>49.66</v>
+        <v>49.81</v>
       </c>
       <c r="G7" t="n">
-        <v>62.85</v>
+        <v>62.86</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.72</v>
+        <v>-0.71</v>
       </c>
       <c r="I7" t="n">
         <v>-0.67</v>
@@ -715,13 +715,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>107702.3</v>
+        <v>107964.61</v>
       </c>
       <c r="E8" t="n">
-        <v>127.18</v>
+        <v>125.87</v>
       </c>
       <c r="F8" t="n">
-        <v>79.72</v>
+        <v>79.73</v>
       </c>
       <c r="G8" t="n">
         <v>82.95999999999999</v>
@@ -749,13 +749,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>76.76000000000001</v>
+        <v>77.41</v>
       </c>
       <c r="E9" t="n">
-        <v>139.9</v>
+        <v>142.4</v>
       </c>
       <c r="F9" t="n">
-        <v>69.95</v>
+        <v>70</v>
       </c>
       <c r="G9" t="n">
         <v>72.12</v>
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>244.23</v>
+        <v>243.67</v>
       </c>
       <c r="E10" t="n">
-        <v>219.96</v>
+        <v>220.06</v>
       </c>
       <c r="F10" t="n">
-        <v>87.09</v>
+        <v>87.06999999999999</v>
       </c>
       <c r="G10" t="n">
         <v>90.81</v>
@@ -817,13 +817,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23.27</v>
+        <v>22.83</v>
       </c>
       <c r="E11" t="n">
-        <v>-117.47</v>
+        <v>-120.8</v>
       </c>
       <c r="F11" t="n">
-        <v>43.12</v>
+        <v>43.07</v>
       </c>
       <c r="G11" t="n">
         <v>42.17</v>
@@ -832,7 +832,7 @@
         <v>-0.11</v>
       </c>
       <c r="I11" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="J11" t="inlineStr"/>
     </row>
@@ -851,10 +851,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1208.15</v>
+        <v>1208.55</v>
       </c>
       <c r="E12" t="n">
-        <v>148.84</v>
+        <v>148.93</v>
       </c>
       <c r="F12" t="n">
         <v>90.87</v>
@@ -885,19 +885,19 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>459.83</v>
+        <v>457.36</v>
       </c>
       <c r="E13" t="n">
-        <v>143.35</v>
+        <v>141.4</v>
       </c>
       <c r="F13" t="n">
-        <v>63.16</v>
+        <v>63.13</v>
       </c>
       <c r="G13" t="n">
         <v>76.86</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.5600000000000001</v>
+        <v>-0.57</v>
       </c>
       <c r="I13" t="n">
         <v>-0.65</v>
@@ -919,13 +919,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>253.36</v>
+        <v>253.65</v>
       </c>
       <c r="E14" t="n">
-        <v>184.03</v>
+        <v>183.8</v>
       </c>
       <c r="F14" t="n">
-        <v>49.16</v>
+        <v>49.17</v>
       </c>
       <c r="G14" t="n">
         <v>52.29</v>
@@ -949,26 +949,26 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>GREE</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>277.42</v>
+        <v>1.51</v>
       </c>
       <c r="E15" t="n">
-        <v>114.83</v>
+        <v>108.79</v>
       </c>
       <c r="F15" t="n">
-        <v>62.22</v>
+        <v>8.24</v>
       </c>
       <c r="G15" t="n">
-        <v>79.55</v>
+        <v>12.81</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.87</v>
+        <v>-0.06</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="J15" t="inlineStr"/>
     </row>
@@ -983,28 +983,62 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GREE</t>
+          <t>DBK.DE</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1.53</v>
+        <v>24.31</v>
       </c>
       <c r="E16" t="n">
-        <v>112.28</v>
+        <v>136.3</v>
       </c>
       <c r="F16" t="n">
-        <v>8.25</v>
+        <v>85.15000000000001</v>
       </c>
       <c r="G16" t="n">
-        <v>12.81</v>
+        <v>85.16</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.06</v>
+        <v>-0.13</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.3</v>
+        <v>0.15</v>
       </c>
       <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45803</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GD</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>277.42</v>
+      </c>
+      <c r="E17" t="n">
+        <v>114.83</v>
+      </c>
+      <c r="F17" t="n">
+        <v>62.22</v>
+      </c>
+      <c r="G17" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-0.87</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1088,26 +1122,26 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>^FTSE</t>
+          <t>GILD</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>8744.559999999999</v>
+        <v>108.44</v>
       </c>
       <c r="E2" t="n">
-        <v>107.32</v>
+        <v>102.73</v>
       </c>
       <c r="F2" t="n">
-        <v>63.21</v>
+        <v>52.26</v>
       </c>
       <c r="G2" t="n">
-        <v>67.06</v>
+        <v>67.69</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01</v>
+        <v>-0.77</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.54</v>
+        <v>-0.63</v>
       </c>
       <c r="J2" t="inlineStr"/>
     </row>
@@ -1122,26 +1156,26 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>^KS11</t>
+          <t>BBAI</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2670.15</v>
+        <v>4.14</v>
       </c>
       <c r="E3" t="n">
-        <v>173.88</v>
+        <v>163.7</v>
       </c>
       <c r="F3" t="n">
-        <v>62.84</v>
+        <v>16.23</v>
       </c>
       <c r="G3" t="n">
-        <v>62.92</v>
+        <v>21.68</v>
       </c>
       <c r="H3" t="n">
-        <v>0.36</v>
+        <v>0.55</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.31</v>
+        <v>-0.92</v>
       </c>
       <c r="J3" t="inlineStr"/>
     </row>
@@ -1156,26 +1190,26 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GILD</t>
+          <t>WBD</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>108.57</v>
+        <v>10.02</v>
       </c>
       <c r="E4" t="n">
-        <v>110.81</v>
+        <v>198.45</v>
       </c>
       <c r="F4" t="n">
-        <v>52.27</v>
+        <v>32.15</v>
       </c>
       <c r="G4" t="n">
-        <v>67.69</v>
+        <v>34.6</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.77</v>
+        <v>-0.18</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.63</v>
+        <v>-0.28</v>
       </c>
       <c r="J4" t="inlineStr"/>
     </row>
@@ -1190,26 +1224,26 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BBAI</t>
+          <t>^FTSE</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4.09</v>
+        <v>8744.559999999999</v>
       </c>
       <c r="E5" t="n">
-        <v>160.79</v>
+        <v>107.32</v>
       </c>
       <c r="F5" t="n">
-        <v>16.2</v>
+        <v>63.21</v>
       </c>
       <c r="G5" t="n">
-        <v>21.68</v>
+        <v>67.06</v>
       </c>
       <c r="H5" t="n">
-        <v>0.55</v>
+        <v>0.01</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.92</v>
+        <v>-0.54</v>
       </c>
       <c r="J5" t="inlineStr"/>
     </row>
@@ -1224,26 +1258,26 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>WBD</t>
+          <t>^KS11</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9.83</v>
+        <v>2670.15</v>
       </c>
       <c r="E6" t="n">
-        <v>168.8</v>
+        <v>173.88</v>
       </c>
       <c r="F6" t="n">
-        <v>32.06</v>
+        <v>62.84</v>
       </c>
       <c r="G6" t="n">
-        <v>34.6</v>
+        <v>62.92</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.19</v>
+        <v>0.36</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.28</v>
+        <v>-0.31</v>
       </c>
       <c r="J6" t="inlineStr"/>
     </row>
@@ -1258,7 +1292,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,41 +1354,41 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45805.5</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AUDUSD=X</t>
+          <t>AUDJPY=X</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.64</v>
+        <v>93.61</v>
       </c>
       <c r="E2" t="n">
-        <v>-111.13</v>
+        <v>190.56</v>
       </c>
       <c r="F2" t="n">
-        <v>51.31</v>
+        <v>30.09</v>
       </c>
       <c r="G2" t="n">
-        <v>48.75</v>
+        <v>36.33</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.39</v>
+        <v>0.53</v>
       </c>
       <c r="I2" t="n">
-        <v>0.19</v>
+        <v>-1</v>
       </c>
       <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45805.5</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1363,32 +1397,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EURUSD=X</t>
+          <t>EURGBP=X</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.13</v>
+        <v>0.84</v>
       </c>
       <c r="E3" t="n">
-        <v>-104.44</v>
+        <v>-127.19</v>
       </c>
       <c r="F3" t="n">
-        <v>70.48</v>
+        <v>21.83</v>
       </c>
       <c r="G3" t="n">
-        <v>54.19</v>
+        <v>19.74</v>
       </c>
       <c r="H3" t="n">
-        <v>0.48</v>
+        <v>0.04</v>
       </c>
       <c r="I3" t="n">
-        <v>1.01</v>
+        <v>0.14</v>
       </c>
       <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45805.5</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1401,28 +1435,28 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>163.67</v>
+        <v>163.97</v>
       </c>
       <c r="E4" t="n">
-        <v>101.23</v>
+        <v>106.02</v>
       </c>
       <c r="F4" t="n">
-        <v>34.74</v>
+        <v>39.81</v>
       </c>
       <c r="G4" t="n">
-        <v>42.61</v>
+        <v>40.24</v>
       </c>
       <c r="H4" t="n">
-        <v>0.21</v>
+        <v>0.8</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.63</v>
+        <v>-0.54</v>
       </c>
       <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45805.5</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1431,32 +1465,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>GBPUSD=X</t>
+          <t>EURCNY=X</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="E5" t="n">
-        <v>-115.83</v>
+        <v>-114.52</v>
       </c>
       <c r="F5" t="n">
-        <v>81.53</v>
+        <v>65.34</v>
       </c>
       <c r="G5" t="n">
-        <v>67.97</v>
+        <v>48.46</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
       <c r="I5" t="n">
-        <v>0.99</v>
+        <v>1.14</v>
       </c>
       <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45805.5</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1465,66 +1499,66 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>USDJPY=X</t>
+          <t>GBPJPY=X</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>144.57</v>
+        <v>195.73</v>
       </c>
       <c r="E6" t="n">
-        <v>107.88</v>
+        <v>114.7</v>
       </c>
       <c r="F6" t="n">
-        <v>27.72</v>
+        <v>47.62</v>
       </c>
       <c r="G6" t="n">
-        <v>43.81</v>
+        <v>50.83</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.31</v>
+        <v>0.51</v>
       </c>
       <c r="I6" t="n">
-        <v>-1</v>
+        <v>-0.64</v>
       </c>
       <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45805.5</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USDILS=X</t>
+          <t>USDJPY=X</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3.51</v>
+        <v>145.36</v>
       </c>
       <c r="E7" t="n">
-        <v>-108.46</v>
+        <v>105.8</v>
       </c>
       <c r="F7" t="n">
-        <v>36.85</v>
+        <v>30.36</v>
       </c>
       <c r="G7" t="n">
-        <v>28.97</v>
+        <v>39.08</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.05</v>
+        <v>0.27</v>
       </c>
       <c r="I7" t="n">
-        <v>0.51</v>
+        <v>-0.99</v>
       </c>
       <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45805.54166666666</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1533,32 +1567,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>^SSMI</t>
+          <t>USDILS=X</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>12199.01</v>
+        <v>3.5</v>
       </c>
       <c r="E8" t="n">
-        <v>-108.22</v>
+        <v>-121.4</v>
       </c>
       <c r="F8" t="n">
-        <v>81.56</v>
+        <v>35.93</v>
       </c>
       <c r="G8" t="n">
-        <v>77.36</v>
+        <v>31.66</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.12</v>
       </c>
       <c r="I8" t="n">
-        <v>0.67</v>
+        <v>0.54</v>
       </c>
       <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45805.39583333334</v>
+        <v>45805.70833333334</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1567,32 +1601,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>LIT</t>
+          <t>^SSMI</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>37.08</v>
+        <v>12196.64</v>
       </c>
       <c r="E9" t="n">
-        <v>-132.36</v>
+        <v>-111.68</v>
       </c>
       <c r="F9" t="n">
-        <v>64.90000000000001</v>
+        <v>80.55</v>
       </c>
       <c r="G9" t="n">
-        <v>49.1</v>
+        <v>77.81</v>
       </c>
       <c r="H9" t="n">
-        <v>0.36</v>
+        <v>-0.15</v>
       </c>
       <c r="I9" t="n">
-        <v>0.97</v>
+        <v>0.63</v>
       </c>
       <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45805.39583333334</v>
+        <v>45805.5625</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1601,32 +1635,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GM</t>
+          <t>LIT</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>48.47</v>
+        <v>36.96</v>
       </c>
       <c r="E10" t="n">
-        <v>-149.89</v>
+        <v>-117.61</v>
       </c>
       <c r="F10" t="n">
-        <v>62.58</v>
+        <v>65.14</v>
       </c>
       <c r="G10" t="n">
-        <v>43.7</v>
+        <v>50.07</v>
       </c>
       <c r="H10" t="n">
-        <v>0.96</v>
+        <v>0.32</v>
       </c>
       <c r="I10" t="n">
-        <v>0.57</v>
+        <v>0.98</v>
       </c>
       <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45805.39583333334</v>
+        <v>45805.5625</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1635,32 +1669,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LYV</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>141.87</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>-119.52</v>
+        <v>-141.03</v>
       </c>
       <c r="F11" t="n">
-        <v>87.22</v>
+        <v>67.58</v>
       </c>
       <c r="G11" t="n">
-        <v>73.89</v>
+        <v>46.84</v>
       </c>
       <c r="H11" t="n">
-        <v>0.32</v>
+        <v>0.9</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>1.09</v>
       </c>
       <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45805.39583333334</v>
+        <v>45805.5</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1669,32 +1703,32 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RIOT</t>
+          <t>NG=F</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>8.48</v>
+        <v>3.19</v>
       </c>
       <c r="E12" t="n">
-        <v>-107.21</v>
+        <v>-162.43</v>
       </c>
       <c r="F12" t="n">
-        <v>67.13</v>
+        <v>30.06</v>
       </c>
       <c r="G12" t="n">
-        <v>46.36</v>
+        <v>29.4</v>
       </c>
       <c r="H12" t="n">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="I12" t="n">
-        <v>1.11</v>
+        <v>-0.58</v>
       </c>
       <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45805.39583333334</v>
+        <v>45805.5625</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1703,62 +1737,810 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BITF</t>
+          <t>STLA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.01</v>
+        <v>10.15</v>
       </c>
       <c r="E13" t="n">
-        <v>-172.7</v>
+        <v>-104.89</v>
       </c>
       <c r="F13" t="n">
-        <v>75.61</v>
+        <v>50.59</v>
       </c>
       <c r="G13" t="n">
-        <v>55.51</v>
+        <v>31.24</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="I13" t="n">
-        <v>1.29</v>
+        <v>0.86</v>
       </c>
       <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
+        <v>45806.33333333334</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MBG.DE</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>53.75</v>
+      </c>
+      <c r="E14" t="n">
+        <v>142.07</v>
+      </c>
+      <c r="F14" t="n">
+        <v>57.76</v>
+      </c>
+      <c r="G14" t="n">
+        <v>65.11</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-0.55</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>48.14</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-152.8</v>
+      </c>
+      <c r="F15" t="n">
+        <v>63.18</v>
+      </c>
+      <c r="G15" t="n">
+        <v>44.51</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>MARA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>14.86</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-168.37</v>
+      </c>
+      <c r="F16" t="n">
+        <v>80.20999999999999</v>
+      </c>
+      <c r="G16" t="n">
+        <v>65.23999999999999</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>LYV</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>140.22</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-175.37</v>
+      </c>
+      <c r="F17" t="n">
+        <v>87.23999999999999</v>
+      </c>
+      <c r="G17" t="n">
+        <v>74.76000000000001</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>8.390000000000001</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-184.05</v>
+      </c>
+      <c r="F18" t="n">
+        <v>68.26000000000001</v>
+      </c>
+      <c r="G18" t="n">
+        <v>47.53</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>HUT</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>15.55</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-141.15</v>
+      </c>
+      <c r="F19" t="n">
+        <v>75.84</v>
+      </c>
+      <c r="G19" t="n">
+        <v>57.68</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CLSK</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>9.119999999999999</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-138.19</v>
+      </c>
+      <c r="F20" t="n">
+        <v>74.47</v>
+      </c>
+      <c r="G20" t="n">
+        <v>61.64</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>BITF</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-221.33</v>
+      </c>
+      <c r="F21" t="n">
+        <v>75.81</v>
+      </c>
+      <c r="G21" t="n">
+        <v>56.72</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45805.5625</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>HIVE</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-106.97</v>
+      </c>
+      <c r="F22" t="n">
+        <v>80.70999999999999</v>
+      </c>
+      <c r="G22" t="n">
+        <v>60.44</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45806.33333333334</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>EURUSD=X</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-100.44</v>
+      </c>
+      <c r="F23" t="n">
+        <v>71.25</v>
+      </c>
+      <c r="G23" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="J23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45805.5</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>AUDUSD=X</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-111.13</v>
+      </c>
+      <c r="F24" t="n">
+        <v>51.31</v>
+      </c>
+      <c r="G24" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="J24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45805.5</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>EURUSD=X</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-104.44</v>
+      </c>
+      <c r="F25" t="n">
+        <v>70.48</v>
+      </c>
+      <c r="G25" t="n">
+        <v>54.19</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="J25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45805.5</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>EURJPY=X</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>163.67</v>
+      </c>
+      <c r="E26" t="n">
+        <v>101.23</v>
+      </c>
+      <c r="F26" t="n">
+        <v>34.74</v>
+      </c>
+      <c r="G26" t="n">
+        <v>42.61</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-0.63</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45805.5</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>GBPUSD=X</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-115.83</v>
+      </c>
+      <c r="F27" t="n">
+        <v>81.53</v>
+      </c>
+      <c r="G27" t="n">
+        <v>67.97</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="J27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45805.5</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>USDJPY=X</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>144.57</v>
+      </c>
+      <c r="E28" t="n">
+        <v>107.88</v>
+      </c>
+      <c r="F28" t="n">
+        <v>27.72</v>
+      </c>
+      <c r="G28" t="n">
+        <v>43.81</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45805.5</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>USDILS=X</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-108.46</v>
+      </c>
+      <c r="F29" t="n">
+        <v>36.85</v>
+      </c>
+      <c r="G29" t="n">
+        <v>28.97</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="J29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45805.54166666666</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>^SSMI</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>12199.01</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-108.22</v>
+      </c>
+      <c r="F30" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="G30" t="n">
+        <v>77.36</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="J30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
         <v>45805.39583333334</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>LIT</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>37.08</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-132.36</v>
+      </c>
+      <c r="F31" t="n">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="G31" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="J31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>48.47</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-149.89</v>
+      </c>
+      <c r="F32" t="n">
+        <v>62.58</v>
+      </c>
+      <c r="G32" t="n">
+        <v>43.7</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="J32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>LYV</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>141.87</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-119.52</v>
+      </c>
+      <c r="F33" t="n">
+        <v>87.22</v>
+      </c>
+      <c r="G33" t="n">
+        <v>73.89</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>RIOT</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-107.21</v>
+      </c>
+      <c r="F34" t="n">
+        <v>67.13</v>
+      </c>
+      <c r="G34" t="n">
+        <v>46.36</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="J34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BITF</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-172.7</v>
+      </c>
+      <c r="F35" t="n">
+        <v>75.61</v>
+      </c>
+      <c r="G35" t="n">
+        <v>55.51</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="J35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45805.39583333334</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
         <is>
           <t>ARBK</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D36" t="n">
         <v>0.4</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E36" t="n">
         <v>-104.58</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F36" t="n">
         <v>66.52</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G36" t="n">
         <v>51.41</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H36" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I36" t="n">
         <v>0.9399999999999999</v>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
token search entry field
</commit_message>
<xml_diff>
--- a/trading_synthesis.xlsx
+++ b/trading_synthesis.xlsx
@@ -698,7 +698,11 @@
       <c r="I7" t="n">
         <v>-0.67</v>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>pas mal bon signal</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -766,7 +770,11 @@
       <c r="I9" t="n">
         <v>-0.21</v>
       </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>tres intéressant jfslfjsljflsjflsjflsjflsjfljslfjslfjslfjlsfjs</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">

</xml_diff>